<commit_message>
Remove venv && update project
</commit_message>
<xml_diff>
--- a/excel_example.xlsx
+++ b/excel_example.xlsx
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="3">
   <si>
+    <t xml:space="preserve">plank</t>
+  </si>
+  <si>
     <t xml:space="preserve">grass</t>
   </si>
   <si>
     <t xml:space="preserve">ground</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plank</t>
   </si>
 </sst>
 </file>
@@ -109,7 +109,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -126,378 +126,378 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AF36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD5" activeCellId="0" sqref="AD5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>0</v>
@@ -512,21 +512,21 @@
         <v>0</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="0" t="s">
         <v>0</v>
       </c>
     </row>
@@ -535,263 +535,263 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>0</v>
@@ -806,1099 +806,1099 @@
         <v>0</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="0" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1909,16 +1909,6 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
@@ -1927,16 +1917,6 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
@@ -1945,16 +1925,6 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
@@ -1963,16 +1933,6 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
@@ -1981,16 +1941,6 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
@@ -1999,16 +1949,6 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
@@ -2017,16 +1957,6 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
@@ -2035,16 +1965,6 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
@@ -2053,16 +1973,6 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
@@ -2071,16 +1981,6 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
@@ -2089,16 +1989,6 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
@@ -2107,16 +1997,6 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
@@ -2125,16 +2005,6 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
@@ -2143,16 +2013,6 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
@@ -2161,16 +2021,6 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
@@ -2179,16 +2029,6 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
@@ -2197,16 +2037,6 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
@@ -2215,16 +2045,6 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>